<commit_message>
added glc concentration to the HPLC file for probe 18,19,20
</commit_message>
<xml_diff>
--- a/data/fermentation raw data/HPLC.xlsx
+++ b/data/fermentation raw data/HPLC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcl./Documents/MATLAB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcl./Documents/ALL /Studium /Master/4. Semester_Thesis/hybrid-model-corynebacterium/data/fermentation raw data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A59F60-6D23-A04A-95B1-AD1D5A23AB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E309DA6-8BCA-DB41-AE9B-2DFE336F2037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29620" yWindow="2540" windowWidth="28040" windowHeight="17440" xr2:uid="{5ABA1AE7-9E6D-F94C-8847-BD666167E2A4}"/>
+    <workbookView xWindow="1040" yWindow="2420" windowWidth="34200" windowHeight="20260" xr2:uid="{5ABA1AE7-9E6D-F94C-8847-BD666167E2A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Time [h]</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Ethanol [g/L]</t>
+  </si>
+  <si>
+    <t>Glucose2 [g/L]</t>
   </si>
 </sst>
 </file>
@@ -110,11 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -431,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8DD3595-F6C5-F84B-9CAA-4C2F7CFB1971}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,406 +446,475 @@
     <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>0.2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>5.22</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>0.16700000000000001</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2">
         <v>7.9000000000000001E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="G2">
+        <v>5.22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2.1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>5.1760000000000002</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>0.16</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>2.7E-2</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>0.104</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="G3">
+        <v>5.1760000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>5.1980000000000004</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>0.11799999999999999</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>0.04</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <v>2E-3</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>0.33400000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="G4">
+        <v>5.1980000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>3.4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>4.6849999999999996</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>0.14099999999999999</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
         <v>0.35699999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="G5">
+        <v>4.6849999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>4.2300000000000004</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>0.187</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6">
         <v>2.4E-2</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>0.14799999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="G6">
+        <v>4.2300000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>5.35</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>3.48</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>0.21</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
         <v>0.14599999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="G7">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>6.35</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>2.8809999999999998</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>0.27600000000000002</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
         <v>0.122</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>0.128</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="G8">
+        <v>2.8809999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>7.3</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>2.0179999999999998</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>0.38100000000000001</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9">
         <v>0.23</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>0.14099999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="G9">
+        <v>2.0179999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>1.5669999999999999</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>0.46700000000000003</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10">
         <v>0.33900000000000002</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="G10">
+        <v>1.5669999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>1.0409999999999999</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>0.42899999999999999</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11">
         <v>0.39</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
         <v>0.156</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="G11">
+        <v>1.0409999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>21.3</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>28.102</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>1.4890000000000001</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
         <v>1.883</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12">
         <v>5.8000000000000003E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="G12">
+        <v>28.102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>23.3</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>34.85</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>1.45</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
         <v>2.0779999999999998</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>4.8000000000000001E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="G13">
+        <v>34.85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
         <v>24.3</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>39.628</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>1.49</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>2.157</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>3.1E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="G14">
+        <v>39.628</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>26.3</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>47.378</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>1.431</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15">
         <v>2.1819999999999999</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15">
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="G15">
+        <v>47.378</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>27.3</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>52.491</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>1.3939999999999999</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>0</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16">
         <v>2.1150000000000002</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16">
         <v>0.153</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="G16">
+        <v>52.491</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>27.9</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>56.664999999999999</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>1.214</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>0</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17">
         <v>1.859</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
         <v>0.20399999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="G17">
+        <v>56.664999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>28.3</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>59.777999999999999</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>0.93799999999999994</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18">
         <v>1.49</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18">
         <v>6.9000000000000006E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+      <c r="G18">
+        <v>59.777999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>30.5</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>68.22</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>0.16300000000000001</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>0.05</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19">
         <v>0.35499999999999998</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>4.1000000000000002E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+      <c r="G19">
+        <v>150.34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>31.5</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20">
         <v>70.64</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20">
         <v>1.2E-2</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20">
         <v>0.122</v>
+      </c>
+      <c r="G20">
+        <v>170.96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>42</v>
+      </c>
+      <c r="G21">
+        <v>120.47499999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>